<commit_message>
update biến toàn cục filepath
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Tài khoản" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>MẬT KHẨU</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -360,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
@@ -386,6 +395,20 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create result page + result item uc
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NGUYEN PHUONG LAN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\C#\LT\ts910\ts910\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C2A1B-4720-4A17-8FE1-30484CF2613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86279A85-DAA3-40EE-91F4-CCB59CD381BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trường thường" sheetId="1" r:id="rId1"/>
@@ -648,10 +648,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.#"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -673,19 +680,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1001,7 +1009,7 @@
   <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1034,130 +1042,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" t="s">
         <v>15</v>
       </c>
@@ -1167,16 +1175,16 @@
       <c r="Q3" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1197,7 +1205,7 @@
       <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>0.7</v>
       </c>
       <c r="H4" t="s">
@@ -1274,7 +1282,7 @@
       <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>0.7</v>
       </c>
       <c r="H5" t="s">
@@ -1351,7 +1359,7 @@
       <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.8</v>
       </c>
       <c r="H6" t="s">
@@ -3563,699 +3571,6 @@
       </c>
       <c r="AA34">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="I1:Q1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA24856-5F79-46EF-A6F1-45B40B96516B}">
-  <dimension ref="A1:AB9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>109</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F4" s="3">
-        <v>100</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="I4" s="3">
-        <v>109</v>
-      </c>
-      <c r="J4" s="3">
-        <v>456</v>
-      </c>
-      <c r="K4" s="3">
-        <v>2022</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="3">
-        <v>105</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="3">
-        <v>36</v>
-      </c>
-      <c r="P4" s="3">
-        <v>36.5</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>26.5</v>
-      </c>
-      <c r="R4" s="3">
-        <v>27</v>
-      </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="X4" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="Z4" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>108</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" s="3">
-        <v>100</v>
-      </c>
-      <c r="G5" s="3">
-        <v>4</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="I5" s="3">
-        <v>108</v>
-      </c>
-      <c r="J5" s="3">
-        <v>417</v>
-      </c>
-      <c r="K5" s="3">
-        <v>2022</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="3">
-        <v>6</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="3">
-        <v>34.25</v>
-      </c>
-      <c r="P5" s="3">
-        <v>34.5</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>26</v>
-      </c>
-      <c r="R5" s="3">
-        <v>26.5</v>
-      </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3">
-        <v>6.95</v>
-      </c>
-      <c r="X5" s="3">
-        <v>6.35</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>6.72</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>30</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="3">
-        <v>100</v>
-      </c>
-      <c r="G6" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" s="3">
-        <v>30</v>
-      </c>
-      <c r="J6" s="3">
-        <v>126</v>
-      </c>
-      <c r="K6" s="3">
-        <v>2022</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="3">
-        <v>35</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="3">
-        <v>27</v>
-      </c>
-      <c r="P6" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="X6" s="3">
-        <v>5.2</v>
-      </c>
-      <c r="Y6" s="3">
-        <v>5.32</v>
-      </c>
-      <c r="Z6" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>55</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="3">
-        <v>100</v>
-      </c>
-      <c r="G7" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I7" s="3">
-        <v>55</v>
-      </c>
-      <c r="J7" s="3">
-        <v>213</v>
-      </c>
-      <c r="K7" s="3">
-        <v>2022</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="3">
-        <v>35</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="3">
-        <v>33</v>
-      </c>
-      <c r="P7" s="3">
-        <v>33.25</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="X7" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="Z7" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>63</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F8" s="3">
-        <v>100</v>
-      </c>
-      <c r="G8" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I8" s="3">
-        <v>63</v>
-      </c>
-      <c r="J8" s="3">
-        <v>258</v>
-      </c>
-      <c r="K8" s="3">
-        <v>2022</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="3">
-        <v>35</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="3">
-        <v>30.75</v>
-      </c>
-      <c r="P8" s="3">
-        <v>31</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3">
-        <v>6.35</v>
-      </c>
-      <c r="X8" s="3">
-        <v>6.05</v>
-      </c>
-      <c r="Y8" s="3">
-        <v>6.18</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AB8" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" s="3">
-        <v>100</v>
-      </c>
-      <c r="G9" s="3">
-        <v>14.5</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="I9" s="3">
-        <v>3</v>
-      </c>
-      <c r="J9" s="3">
-        <v>21</v>
-      </c>
-      <c r="K9" s="3">
-        <v>2022</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="3">
-        <v>35</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="3">
-        <v>27.5</v>
-      </c>
-      <c r="P9" s="3">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
-      <c r="V9" s="3">
-        <v>0</v>
-      </c>
-      <c r="W9" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="X9" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="Y9" s="3">
-        <v>4.93</v>
-      </c>
-      <c r="Z9" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB9" s="3">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4269,8 +3584,687 @@
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="I1:Q1"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA24856-5F79-46EF-A6F1-45B40B96516B}">
+  <dimension ref="A1:AB9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
+    <col min="27" max="27" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" t="s">
+        <v>156</v>
+      </c>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>1.2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4">
+        <v>109</v>
+      </c>
+      <c r="J4">
+        <v>456</v>
+      </c>
+      <c r="K4">
+        <v>2022</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4">
+        <v>105</v>
+      </c>
+      <c r="N4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4">
+        <v>36</v>
+      </c>
+      <c r="P4">
+        <v>36.5</v>
+      </c>
+      <c r="Q4">
+        <v>26.5</v>
+      </c>
+      <c r="R4">
+        <v>27</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>7.4</v>
+      </c>
+      <c r="X4">
+        <v>6.7</v>
+      </c>
+      <c r="Y4">
+        <v>7.1</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I5">
+        <v>108</v>
+      </c>
+      <c r="J5">
+        <v>417</v>
+      </c>
+      <c r="K5">
+        <v>2022</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>34.25</v>
+      </c>
+      <c r="P5">
+        <v>34.5</v>
+      </c>
+      <c r="Q5">
+        <v>26</v>
+      </c>
+      <c r="R5">
+        <v>26.5</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>6.95</v>
+      </c>
+      <c r="X5">
+        <v>6.35</v>
+      </c>
+      <c r="Y5">
+        <v>6.72</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>4.5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>126</v>
+      </c>
+      <c r="K6">
+        <v>2022</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6">
+        <v>27</v>
+      </c>
+      <c r="P6">
+        <v>27.5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>159</v>
+      </c>
+      <c r="R6" t="s">
+        <v>159</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>5.4</v>
+      </c>
+      <c r="X6">
+        <v>5.2</v>
+      </c>
+      <c r="Y6">
+        <v>5.32</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7">
+        <v>55</v>
+      </c>
+      <c r="J7">
+        <v>213</v>
+      </c>
+      <c r="K7">
+        <v>2022</v>
+      </c>
+      <c r="L7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7">
+        <v>33</v>
+      </c>
+      <c r="P7">
+        <v>33.25</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>159</v>
+      </c>
+      <c r="R7" t="s">
+        <v>159</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>6.7</v>
+      </c>
+      <c r="X7">
+        <v>6.2</v>
+      </c>
+      <c r="Y7">
+        <v>6.5</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>7.1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I8">
+        <v>63</v>
+      </c>
+      <c r="J8">
+        <v>258</v>
+      </c>
+      <c r="K8">
+        <v>2022</v>
+      </c>
+      <c r="L8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8">
+        <v>30.75</v>
+      </c>
+      <c r="P8">
+        <v>31</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>159</v>
+      </c>
+      <c r="R8" t="s">
+        <v>159</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>6.35</v>
+      </c>
+      <c r="X8">
+        <v>6.05</v>
+      </c>
+      <c r="Y8">
+        <v>6.18</v>
+      </c>
+      <c r="Z8">
+        <v>2</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>14.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>180</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>21</v>
+      </c>
+      <c r="K9">
+        <v>2022</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9">
+        <v>27.5</v>
+      </c>
+      <c r="P9">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>159</v>
+      </c>
+      <c r="R9" t="s">
+        <v>159</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>5.5</v>
+      </c>
+      <c r="X9">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y9">
+        <v>4.93</v>
+      </c>
+      <c r="Z9">
+        <v>2</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U3"/>
@@ -4279,14 +4273,21 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AA4" r:id="rId1" xr:uid="{D334F06D-47DD-4266-A1AE-4470382530DD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4306,649 +4307,647 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" t="s">
         <v>156</v>
       </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4">
         <v>109</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>1.2</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>160</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4">
         <v>109</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4">
         <v>462</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4">
         <v>2022</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4">
         <v>70</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4">
         <v>38.25</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4">
         <v>39</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4">
         <v>26.5</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4">
         <v>27</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3">
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <v>7.65</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4">
         <v>7</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4">
         <v>7.35</v>
       </c>
-      <c r="Z4" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA4" s="3" t="s">
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4" t="s">
         <v>161</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AB4">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5">
         <v>108</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>164</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>108</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <v>420</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <v>2022</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5">
         <v>35</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5">
         <v>37.75</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5">
         <v>38</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5">
         <v>26</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5">
         <v>26.5</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <v>7.55</v>
       </c>
-      <c r="X5" s="3">
+      <c r="X5">
         <v>6.85</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Y5">
         <v>7.22</v>
       </c>
-      <c r="Z5" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="3" t="s">
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5" t="s">
         <v>165</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AB5">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6">
         <v>30</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>166</v>
       </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" t="s">
         <v>167</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>4.5</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" t="s">
         <v>168</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <v>30</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <v>129</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <v>2022</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6">
         <v>35</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6">
         <v>34</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6">
         <v>34.5</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" t="s">
         <v>159</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="R6" t="s">
         <v>159</v>
       </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>6.8</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6">
         <v>5.6</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6">
         <v>6.25</v>
       </c>
-      <c r="Z6" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA6" s="3" t="s">
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6" t="s">
         <v>169</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7">
         <v>55</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" t="s">
         <v>171</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>172</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <v>55</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <v>216</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <v>2022</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7">
         <v>35</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7">
         <v>36.25</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7">
         <v>37.25</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q7" t="s">
         <v>159</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="R7" t="s">
         <v>159</v>
       </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="3">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
         <v>7.25</v>
       </c>
-      <c r="X7" s="3">
+      <c r="X7">
         <v>6.75</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="Y7">
         <v>7</v>
       </c>
-      <c r="Z7" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="3" t="s">
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7" t="s">
         <v>173</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AB7">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8">
         <v>63</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>175</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>100</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>7.1</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>176</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8">
         <v>63</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <v>261</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <v>2022</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8">
         <v>35</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8">
         <v>35.5</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8">
         <v>35.5</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" t="s">
         <v>159</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" t="s">
         <v>159</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
-      <c r="V8" s="3">
-        <v>0</v>
-      </c>
-      <c r="W8" s="3">
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <v>7.1</v>
       </c>
-      <c r="X8" s="3">
+      <c r="X8">
         <v>6.55</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8">
         <v>6.77</v>
       </c>
-      <c r="Z8" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA8" s="3" t="s">
+      <c r="Z8">
+        <v>2</v>
+      </c>
+      <c r="AA8" t="s">
         <v>177</v>
       </c>
-      <c r="AB8" s="3">
+      <c r="AB8">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>10</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" t="s">
         <v>179</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>100</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>14.5</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>180</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <v>24</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9">
         <v>2022</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9">
         <v>35</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="N9" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9">
         <v>33.25</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9">
         <v>34.25</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="Q9" t="s">
         <v>159</v>
       </c>
-      <c r="R9" s="3" t="s">
+      <c r="R9" t="s">
         <v>159</v>
       </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
-      <c r="V9" s="3">
-        <v>0</v>
-      </c>
-      <c r="W9" s="3">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
         <v>6.65</v>
       </c>
-      <c r="X9" s="3">
+      <c r="X9">
         <v>5.95</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9">
         <v>6.2</v>
       </c>
-      <c r="Z9" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA9" s="3" t="s">
+      <c r="Z9">
+        <v>2</v>
+      </c>
+      <c r="AA9" t="s">
         <v>181</v>
       </c>
-      <c r="AB9" s="3">
+      <c r="AB9">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="S1:S3"/>
     <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="I2:I3"/>
@@ -4964,17 +4963,7 @@
     <mergeCell ref="X1:X3"/>
     <mergeCell ref="Y1:Y3"/>
     <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5000,842 +4989,820 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="4" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4">
         <v>109</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4">
         <v>100</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <v>1.2</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" t="s">
         <v>160</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4">
         <v>109</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4">
         <v>468</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4">
         <v>2022</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4">
         <v>70</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4">
         <v>34.5</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4">
         <v>35</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4">
-        <v>0</v>
-      </c>
-      <c r="T4" s="4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="4">
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <v>8.6199999999999992</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4">
         <v>8.25</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4">
         <v>8.4700000000000006</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4">
         <v>3</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" t="s">
         <v>161</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z4">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <v>16</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5">
         <v>72</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5">
         <v>2022</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5">
         <v>70</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5">
         <v>32</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5">
         <v>32.25</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4">
-        <v>0</v>
-      </c>
-      <c r="T5" s="4">
-        <v>0</v>
-      </c>
-      <c r="U5" s="4">
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <v>8</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5">
         <v>6.2</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5">
         <v>7.1</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5">
         <v>3</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Y5" t="s">
         <v>65</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z5">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <v>2.4</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>6</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6">
         <v>2022</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6">
         <v>105</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6">
         <v>29.5</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6">
         <v>29.75</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4">
-        <v>0</v>
-      </c>
-      <c r="T6" s="4">
-        <v>0</v>
-      </c>
-      <c r="U6" s="4">
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <v>7.38</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6">
         <v>5.2</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6">
         <v>6.23</v>
       </c>
-      <c r="X6" s="4">
+      <c r="X6">
         <v>3</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="Y6" t="s">
         <v>69</v>
       </c>
-      <c r="Z6" s="4">
+      <c r="Z6">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="4">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" t="s">
         <v>92</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <v>2.9</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" t="s">
         <v>93</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <v>21</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>87</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7">
         <v>2022</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7">
         <v>35</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7">
         <v>32.25</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7">
         <v>33.25</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4">
-        <v>0</v>
-      </c>
-      <c r="U7" s="4">
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <v>8.06</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7">
         <v>6.7</v>
       </c>
-      <c r="W7" s="4">
+      <c r="W7">
         <v>7.38</v>
       </c>
-      <c r="X7" s="4">
+      <c r="X7">
         <v>3</v>
       </c>
-      <c r="Y7" s="4" t="s">
+      <c r="Y7" t="s">
         <v>94</v>
       </c>
-      <c r="Z7" s="4">
+      <c r="Z7">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8">
         <v>108</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>162</v>
       </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8">
         <v>100</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8">
         <v>4</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" t="s">
         <v>164</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <v>108</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <v>426</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8">
         <v>2022</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8">
         <v>105</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8">
         <v>34.25</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8">
         <v>34.5</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4">
-        <v>0</v>
-      </c>
-      <c r="T8" s="4">
-        <v>0</v>
-      </c>
-      <c r="U8" s="4">
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
         <v>8.56</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8">
         <v>8.1</v>
       </c>
-      <c r="W8" s="4">
+      <c r="W8">
         <v>8.3000000000000007</v>
       </c>
-      <c r="X8" s="4">
+      <c r="X8">
         <v>3</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="Y8" t="s">
         <v>165</v>
       </c>
-      <c r="Z8" s="4">
+      <c r="Z8">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9">
         <v>55</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>10</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>171</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9">
         <v>98</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" t="s">
         <v>172</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9">
         <v>55</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9">
         <v>222</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9">
         <v>2022</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9">
         <v>105</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9">
         <v>31</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9">
         <v>31</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4">
-        <v>0</v>
-      </c>
-      <c r="T9" s="4">
-        <v>0</v>
-      </c>
-      <c r="U9" s="4">
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
         <v>7.75</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9">
         <v>5.6</v>
       </c>
-      <c r="W9" s="4">
+      <c r="W9">
         <v>6.52</v>
       </c>
-      <c r="X9" s="4">
+      <c r="X9">
         <v>3</v>
       </c>
-      <c r="Y9" s="4" t="s">
+      <c r="Y9" t="s">
         <v>173</v>
       </c>
-      <c r="Z9" s="4">
+      <c r="Z9">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10">
         <v>68</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>10</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10">
         <v>92</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10">
         <v>6.1</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" t="s">
         <v>154</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10">
         <v>68</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>285</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10">
         <v>2022</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10">
         <v>105</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="N10" t="s">
         <v>32</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10">
         <v>29.5</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10">
         <v>30</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
-        <v>0</v>
-      </c>
-      <c r="U10" s="4">
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <v>7.38</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10">
         <v>4</v>
       </c>
-      <c r="W10" s="4">
+      <c r="W10">
         <v>5.26</v>
       </c>
-      <c r="X10" s="4">
+      <c r="X10">
         <v>3</v>
       </c>
-      <c r="Y10" s="4" t="s">
+      <c r="Y10" t="s">
         <v>155</v>
       </c>
-      <c r="Z10" s="4">
+      <c r="Z10">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11">
         <v>63</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="4">
-        <v>2</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>100</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11">
         <v>7.1</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" t="s">
         <v>176</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11">
         <v>63</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <v>267</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11">
         <v>2022</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11">
         <v>105</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11">
         <v>31.25</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11">
         <v>31.5</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4">
-        <v>0</v>
-      </c>
-      <c r="T11" s="4">
-        <v>0</v>
-      </c>
-      <c r="U11" s="4">
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
         <v>7.8100000000000005</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11">
         <v>7</v>
       </c>
-      <c r="W11" s="4">
+      <c r="W11">
         <v>7.34</v>
       </c>
-      <c r="X11" s="4">
+      <c r="X11">
         <v>3</v>
       </c>
-      <c r="Y11" s="4" t="s">
+      <c r="Y11" t="s">
         <v>177</v>
       </c>
-      <c r="Z11" s="4">
+      <c r="Z11">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
+      <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>178</v>
       </c>
-      <c r="C12" s="4">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>179</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12">
         <v>100</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12">
         <v>14.5</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" t="s">
         <v>180</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12">
         <v>3</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12">
         <v>30</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12">
         <v>2022</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12">
         <v>70</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="N12" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12">
         <v>26.5</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12">
         <v>26.75</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4">
-        <v>0</v>
-      </c>
-      <c r="T12" s="4">
-        <v>0</v>
-      </c>
-      <c r="U12" s="4">
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
         <v>6.62</v>
       </c>
-      <c r="V12" s="4">
+      <c r="V12">
         <v>4.8</v>
       </c>
-      <c r="W12" s="4">
+      <c r="W12">
         <v>5.71</v>
       </c>
-      <c r="X12" s="4">
+      <c r="X12">
         <v>3</v>
       </c>
-      <c r="Y12" s="4" t="s">
+      <c r="Y12" t="s">
         <v>181</v>
       </c>
-      <c r="Z12" s="4">
+      <c r="Z12">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:S3"/>
@@ -5844,13 +5811,17 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5860,61 +5831,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3E9D1D-7468-4015-944B-4DBA3923072B}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>189</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>193</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sửa UI đăng ký, đăng nhập, pop up tư vấn
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\C#\LT\ts910\ts910\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Oanhhh\c#\ts910\ts910\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86279A85-DAA3-40EE-91F4-CCB59CD381BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trường thường" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="194">
   <si>
     <t>highschoolid</t>
   </si>
@@ -620,31 +619,28 @@
     <t>MẬT KHẨU</t>
   </si>
   <si>
+    <t>SỐ ĐIỆN THOẠI</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>lan</t>
-  </si>
-  <si>
-    <t>lan2205</t>
+    <t>hoangoanh</t>
+  </si>
+  <si>
+    <t>oanh@gm.com</t>
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>12bc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.#"/>
   </numFmts>
@@ -687,10 +683,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1005,7 +1001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7EFDBE-1BAF-4FC3-98AE-9C145D90626F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1042,130 +1038,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
       <c r="O3" t="s">
         <v>15</v>
       </c>
@@ -1175,16 +1171,16 @@
       <c r="Q3" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -3607,10 +3603,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA24856-5F79-46EF-A6F1-45B40B96516B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -3627,132 +3623,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
       <c r="O3" t="s">
         <v>15</v>
       </c>
@@ -3765,16 +3761,16 @@
       <c r="R3" t="s">
         <v>156</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -3849,7 +3845,7 @@
       <c r="Z4">
         <v>2</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="AB4">
@@ -4286,14 +4282,14 @@
     <mergeCell ref="E1:E3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AA4" r:id="rId1" xr:uid="{D334F06D-47DD-4266-A1AE-4470382530DD}"/>
+    <hyperlink ref="AA4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B140F43-8AF7-4427-8710-A095BAD2D5C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4307,132 +4303,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
       <c r="O3" t="s">
         <v>15</v>
       </c>
@@ -4445,16 +4441,16 @@
       <c r="R3" t="s">
         <v>156</v>
       </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -4970,7 +4966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF43877-1FF0-4D57-A333-9DBE4174D065}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4989,144 +4985,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
       <c r="O3" t="s">
         <v>15</v>
       </c>
       <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -5828,16 +5824,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3E9D1D-7468-4015-944B-4DBA3923072B}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>182</v>
       </c>
@@ -5848,41 +5847,36 @@
         <v>184</v>
       </c>
       <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" t="s">
         <v>185</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>186</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
         <v>191</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D2" t="s">
         <v>192</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E2" t="s">
         <v>193</v>
       </c>
-      <c r="F3" t="s">
-        <v>194</v>
+      <c r="G2" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
load data from excel file
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Oanhhh\c#\ts910\ts910\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\C#\LT\ts910\ts910\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E882ABEA-E274-4CC7-821C-1A264E331444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="3855" yWindow="3270" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trường thường" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="196">
   <si>
     <t>highschoolid</t>
   </si>
@@ -635,12 +636,18 @@
   </si>
   <si>
     <t>12bc</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>lan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.#"/>
   </numFmts>
@@ -1001,7 +1008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3571,11 +3578,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
@@ -3587,32 +3599,27 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F10" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" customWidth="1"/>
@@ -4254,13 +4261,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U3"/>
@@ -4269,30 +4280,26 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="AA4" r:id="rId1"/>
+    <hyperlink ref="AA4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -4934,16 +4941,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="S1:S3"/>
     <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="I2:I3"/>
@@ -4960,13 +4957,23 @@
     <mergeCell ref="Y1:Y3"/>
     <mergeCell ref="Z1:Z3"/>
     <mergeCell ref="T1:T3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5792,13 +5799,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:S3"/>
@@ -5807,32 +5818,29 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5866,7 +5874,7 @@
       <c r="B2" t="s">
         <v>190</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>191</v>
       </c>
       <c r="D2" t="s">
@@ -5879,7 +5887,30 @@
         <v>192</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1A7A8B47-41E8-4D54-86E3-460B11C9C068}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa giao diện, ghép socket với app
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3270" windowWidth="21600" windowHeight="11385" activeTab="4"/>
+    <workbookView xWindow="3855" yWindow="3270" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trường thường" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="202">
   <si>
     <t>highschoolid</t>
   </si>
@@ -644,6 +644,21 @@
   </si>
   <si>
     <t>Resources/user.png</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0a</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -3580,11 +3595,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
@@ -3596,16 +3616,11 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4263,13 +4278,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U3"/>
@@ -4278,17 +4297,13 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA4" r:id="rId1"/>
@@ -4943,16 +4958,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="S1:S3"/>
     <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="I2:I3"/>
@@ -4969,6 +4974,16 @@
     <mergeCell ref="Y1:Y3"/>
     <mergeCell ref="Z1:Z3"/>
     <mergeCell ref="T1:T3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5801,13 +5816,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:S3"/>
@@ -5816,17 +5835,13 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5834,7 +5849,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -5915,6 +5930,29 @@
         <v>192</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
update doi mat khau
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="202">
   <si>
     <t>highschoolid</t>
   </si>
@@ -3595,16 +3595,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
@@ -3616,11 +3611,16 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4278,17 +4278,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U3"/>
@@ -4297,13 +4293,17 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA4" r:id="rId1"/>
@@ -4958,6 +4958,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="S1:S3"/>
     <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="I2:I3"/>
@@ -4974,16 +4984,6 @@
     <mergeCell ref="Y1:Y3"/>
     <mergeCell ref="Z1:Z3"/>
     <mergeCell ref="T1:T3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5816,17 +5816,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:S3"/>
@@ -5835,13 +5831,17 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I1:P1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5926,8 +5926,8 @@
       <c r="F3" t="s">
         <v>196</v>
       </c>
-      <c r="G3" t="s">
-        <v>192</v>
+      <c r="G3">
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update thay doi thong tin
</commit_message>
<xml_diff>
--- a/ts910/data.xlsx
+++ b/ts910/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="205">
   <si>
     <t>highschoolid</t>
   </si>
@@ -659,6 +659,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>123a</t>
+  </si>
+  <si>
+    <t>lannn</t>
+  </si>
+  <si>
+    <t>G:\Oanhhh\picture\pencil.png</t>
   </si>
 </sst>
 </file>
@@ -3595,11 +3604,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
@@ -3611,16 +3625,11 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4278,13 +4287,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="AA1:AA3"/>
-    <mergeCell ref="AB1:AB3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U3"/>
@@ -4293,17 +4306,13 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="AA1:AA3"/>
+    <mergeCell ref="AB1:AB3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA4" r:id="rId1"/>
@@ -4958,16 +4967,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:R1"/>
-    <mergeCell ref="S1:S3"/>
     <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="AB1:AB3"/>
     <mergeCell ref="I2:I3"/>
@@ -4984,6 +4983,16 @@
     <mergeCell ref="Y1:Y3"/>
     <mergeCell ref="Z1:Z3"/>
     <mergeCell ref="T1:T3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5816,13 +5825,17 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Y1:Y3"/>
-    <mergeCell ref="Z1:Z3"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="V1:V3"/>
-    <mergeCell ref="W1:W3"/>
-    <mergeCell ref="X1:X3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:Q3"/>
     <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:S3"/>
@@ -5831,17 +5844,13 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="I1:P1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="Y1:Y3"/>
+    <mergeCell ref="Z1:Z3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="X1:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5912,22 +5921,22 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" t="s">
-        <v>192</v>
+      <c r="D3">
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="G3">
-        <v>123</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>